<commit_message>
Change basic pytests that ensure that simulation does not terminate
- Change `tests/test_basic.py`:
    - Remove pytests for black, as they do not work
    - Update `test_execution_not_terminated`
- Update `tests/inputs/pytest_test.xlsx`
</commit_message>
<xml_diff>
--- a/tests/inputs/pytest_test.xlsx
+++ b/tests/inputs/pytest_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="346">
   <si>
     <t>Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -1091,7 +1091,10 @@
     <t>show</t>
   </si>
   <si>
-    <t>simulation_results</t>
+    <t>genset_with_efficiency_curve</t>
+  </si>
+  <si>
+    <t>oem, string (name of base capacity case), None, peak_demand</t>
   </si>
 </sst>
 </file>
@@ -1402,39 +1405,6 @@
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1591,6 +1561,39 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1957,179 +1960,179 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="17" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="17" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="17" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2149,121 +2152,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.08984375" customWidth="1"/>
     <col min="2" max="2" width="33.36328125" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="9" customWidth="1"/>
     <col min="4" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2271,7 +2274,7 @@
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2279,7 +2282,7 @@
       <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2287,7 +2290,7 @@
       <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2295,7 +2298,7 @@
       <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2303,7 +2306,7 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="16">
         <v>7</v>
       </c>
     </row>
@@ -2311,7 +2314,7 @@
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="17">
         <v>43101</v>
       </c>
     </row>
@@ -2319,7 +2322,7 @@
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D19" t="s">
@@ -2330,7 +2333,7 @@
       <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2338,24 +2341,24 @@
       <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="29"/>
+      <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2363,7 +2366,7 @@
       <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2371,7 +2374,7 @@
       <c r="B26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D26" t="s">
@@ -2382,25 +2385,25 @@
       <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="16">
         <v>0.03</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="29"/>
+      <c r="C28" s="18"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="19"/>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
+      <c r="A30" s="10"/>
       <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D30" t="s">
@@ -2408,39 +2411,39 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
+      <c r="A31" s="10"/>
       <c r="B31" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>344</v>
+      <c r="C31" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="A32" s="10"/>
       <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="30"/>
+      <c r="C33" s="19"/>
     </row>
     <row r="34" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="32"/>
-      <c r="G34" s="32"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="21"/>
+      <c r="G34" s="21"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2448,7 +2451,7 @@
       <c r="B36" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D36" t="s">
@@ -2459,7 +2462,7 @@
       <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2467,7 +2470,7 @@
       <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2475,7 +2478,7 @@
       <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2483,7 +2486,7 @@
       <c r="B40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2491,25 +2494,25 @@
       <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="26" t="s">
-        <v>41</v>
+      <c r="C41" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="30"/>
+      <c r="C42" s="19"/>
     </row>
     <row r="43" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="30"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="19"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2517,7 +2520,7 @@
       <c r="B45" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2525,24 +2528,24 @@
       <c r="B46" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="30"/>
+      <c r="C47" s="19"/>
     </row>
     <row r="48" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="29"/>
+      <c r="C48" s="18"/>
     </row>
     <row r="49" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2550,7 +2553,7 @@
       <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2558,7 +2561,7 @@
       <c r="B51" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2566,7 +2569,7 @@
       <c r="B52" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2600,67 +2603,67 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="22" customWidth="1"/>
     <col min="4" max="1023" width="8.6328125" customWidth="1"/>
     <col min="1024" max="1025" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:7" ht="46.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="25" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2668,10 +2671,10 @@
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="16">
         <v>0</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="13" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2679,10 +2682,10 @@
       <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="16">
         <v>0</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2690,10 +2693,10 @@
       <c r="A9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="16">
         <v>0</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="13" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2701,10 +2704,10 @@
       <c r="A10" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="16">
         <v>0</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2712,10 +2715,10 @@
       <c r="A11" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="16">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2723,10 +2726,10 @@
       <c r="A12" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="16">
         <v>1</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2734,10 +2737,10 @@
       <c r="A13" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2745,10 +2748,10 @@
       <c r="A14" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="16">
         <v>0</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2756,10 +2759,10 @@
       <c r="A15" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="16">
         <v>0</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2767,10 +2770,10 @@
       <c r="A16" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="16">
         <v>40</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2778,10 +2781,10 @@
       <c r="A17" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="16">
         <v>0.5</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2789,10 +2792,10 @@
       <c r="A18" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="16">
         <v>820</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2800,10 +2803,10 @@
       <c r="A19" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="16">
         <v>0.05</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2811,10 +2814,10 @@
       <c r="A20" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="16">
         <v>0</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2822,10 +2825,10 @@
       <c r="A21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="16">
         <v>0.33</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2833,10 +2836,10 @@
       <c r="A22" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="16">
         <v>10</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2844,10 +2847,10 @@
       <c r="A23" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="16">
         <v>1</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2855,10 +2858,10 @@
       <c r="A24" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="16">
         <v>0.1</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2866,10 +2869,10 @@
       <c r="A25" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="16">
         <v>1</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D25" t="s">
@@ -2880,10 +2883,10 @@
       <c r="A26" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="16">
         <v>0.5</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2891,10 +2894,10 @@
       <c r="A27" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="16">
         <v>0</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2902,10 +2905,10 @@
       <c r="A28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="16">
         <v>0</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2913,10 +2916,10 @@
       <c r="A29" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="16">
         <v>0</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2924,10 +2927,10 @@
       <c r="A30" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="9">
         <v>1</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2935,10 +2938,10 @@
       <c r="A31" t="s">
         <v>125</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="9">
         <v>15</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2946,10 +2949,10 @@
       <c r="A32" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="16">
         <v>1</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2957,10 +2960,10 @@
       <c r="A33" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="16">
         <v>0.08</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2968,10 +2971,10 @@
       <c r="A34" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="16">
         <v>0</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="13" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2979,10 +2982,10 @@
       <c r="A35" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="16">
         <v>0</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="13" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2990,10 +2993,10 @@
       <c r="A36" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="16">
         <v>40</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="13" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3001,10 +3004,10 @@
       <c r="A37" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="16">
         <v>0.05</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3012,10 +3015,10 @@
       <c r="A38" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="16">
         <v>0</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3023,10 +3026,10 @@
       <c r="A39" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="16">
         <v>0</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3034,10 +3037,10 @@
       <c r="A40" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="27">
+      <c r="B40" s="16">
         <v>1</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3045,10 +3048,10 @@
       <c r="A41" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="27">
+      <c r="B41" s="16">
         <v>200</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3056,10 +3059,10 @@
       <c r="A42" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B42" s="16">
         <v>0</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3067,10 +3070,10 @@
       <c r="A43" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="16">
         <v>0</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3078,10 +3081,10 @@
       <c r="A44" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="16">
         <v>1</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3089,10 +3092,10 @@
       <c r="A45" t="s">
         <v>142</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="16">
         <v>20</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3100,10 +3103,10 @@
       <c r="A46" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="27">
+      <c r="B46" s="16">
         <v>1.5</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D46" t="s">
@@ -3114,10 +3117,10 @@
       <c r="A47" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="27">
+      <c r="B47" s="16">
         <v>0.68</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="13" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3125,10 +3128,10 @@
       <c r="A48" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="16">
         <v>0.05</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="13" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3136,10 +3139,10 @@
       <c r="A49" t="s">
         <v>148</v>
       </c>
-      <c r="B49" s="27">
+      <c r="B49" s="16">
         <v>20000</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3147,10 +3150,10 @@
       <c r="A50" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="27">
+      <c r="B50" s="16">
         <v>0</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3158,10 +3161,10 @@
       <c r="A51" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="27">
+      <c r="B51" s="16">
         <v>20</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3169,10 +3172,10 @@
       <c r="A52" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="27">
+      <c r="B52" s="16">
         <v>0.5</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="13" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3180,10 +3183,10 @@
       <c r="A53" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="27">
+      <c r="B53" s="16">
         <v>1250</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="13" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3191,10 +3194,10 @@
       <c r="A54" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="27">
+      <c r="B54" s="16">
         <v>25</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="13" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3202,10 +3205,10 @@
       <c r="A55" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="27">
+      <c r="B55" s="16">
         <v>0</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3213,10 +3216,10 @@
       <c r="A56" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="27">
+      <c r="B56" s="16">
         <v>25</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3224,10 +3227,10 @@
       <c r="A57" t="s">
         <v>159</v>
       </c>
-      <c r="B57" s="27">
+      <c r="B57" s="16">
         <v>0.5</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3235,10 +3238,10 @@
       <c r="A58" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="27">
+      <c r="B58" s="16">
         <v>0</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3246,10 +3249,10 @@
       <c r="A59" t="s">
         <v>161</v>
       </c>
-      <c r="B59" s="27">
+      <c r="B59" s="16">
         <v>0</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3257,10 +3260,10 @@
       <c r="A60" t="s">
         <v>162</v>
       </c>
-      <c r="B60" s="27">
+      <c r="B60" s="16">
         <v>0</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3268,10 +3271,10 @@
       <c r="A61" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B61" s="9">
         <v>1</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C61" s="22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3279,10 +3282,10 @@
       <c r="A62" t="s">
         <v>164</v>
       </c>
-      <c r="B62" s="20">
+      <c r="B62" s="9">
         <v>15</v>
       </c>
-      <c r="C62" s="33" t="s">
+      <c r="C62" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3290,10 +3293,10 @@
       <c r="A63" t="s">
         <v>165</v>
       </c>
-      <c r="B63" s="27">
+      <c r="B63" s="16">
         <v>0</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3301,10 +3304,10 @@
       <c r="A64" t="s">
         <v>166</v>
       </c>
-      <c r="B64" s="27">
+      <c r="B64" s="16">
         <v>1</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3312,10 +3315,10 @@
       <c r="A65" t="s">
         <v>167</v>
       </c>
-      <c r="B65" s="27">
+      <c r="B65" s="16">
         <v>0.5</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3323,10 +3326,10 @@
       <c r="A66" t="s">
         <v>168</v>
       </c>
-      <c r="B66" s="27">
+      <c r="B66" s="16">
         <v>0.2</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3334,10 +3337,10 @@
       <c r="A67" t="s">
         <v>169</v>
       </c>
-      <c r="B67" s="27">
+      <c r="B67" s="16">
         <v>1</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="13" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3345,10 +3348,10 @@
       <c r="A68" t="s">
         <v>171</v>
       </c>
-      <c r="B68" s="27">
+      <c r="B68" s="16">
         <v>1</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="13" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3356,10 +3359,10 @@
       <c r="A69" t="s">
         <v>172</v>
       </c>
-      <c r="B69" s="27">
+      <c r="B69" s="16">
         <v>250</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3367,10 +3370,10 @@
       <c r="A70" t="s">
         <v>173</v>
       </c>
-      <c r="B70" s="27">
+      <c r="B70" s="16">
         <v>6.75</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="13" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3378,10 +3381,10 @@
       <c r="A71" t="s">
         <v>175</v>
       </c>
-      <c r="B71" s="27">
+      <c r="B71" s="16">
         <v>13.5</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3389,10 +3392,10 @@
       <c r="A72" t="s">
         <v>176</v>
       </c>
-      <c r="B72" s="27">
+      <c r="B72" s="16">
         <v>0</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3400,10 +3403,10 @@
       <c r="A73" t="s">
         <v>177</v>
       </c>
-      <c r="B73" s="27">
+      <c r="B73" s="16">
         <v>1</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3411,10 +3414,10 @@
       <c r="A74" t="s">
         <v>178</v>
       </c>
-      <c r="B74" s="37">
+      <c r="B74" s="26">
         <v>0.5</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3422,10 +3425,10 @@
       <c r="A75" t="s">
         <v>179</v>
       </c>
-      <c r="B75" s="27">
+      <c r="B75" s="16">
         <v>0.97</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3433,10 +3436,10 @@
       <c r="A76" t="s">
         <v>180</v>
       </c>
-      <c r="B76" s="27">
+      <c r="B76" s="16">
         <v>0.97</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C76" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3444,10 +3447,10 @@
       <c r="A77" t="s">
         <v>181</v>
       </c>
-      <c r="B77" s="27">
+      <c r="B77" s="16">
         <v>0</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C77" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3455,10 +3458,10 @@
       <c r="A78" t="s">
         <v>182</v>
       </c>
-      <c r="B78" s="27">
+      <c r="B78" s="16">
         <v>500</v>
       </c>
-      <c r="C78" s="24" t="s">
+      <c r="C78" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3466,10 +3469,10 @@
       <c r="A79" t="s">
         <v>183</v>
       </c>
-      <c r="B79" s="27">
+      <c r="B79" s="16">
         <v>0</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3477,10 +3480,10 @@
       <c r="A80" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="27">
+      <c r="B80" s="16">
         <v>13.5</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C80" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3488,10 +3491,10 @@
       <c r="A81" t="s">
         <v>185</v>
       </c>
-      <c r="B81" s="27" t="s">
+      <c r="B81" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C81" s="24" t="s">
+      <c r="C81" s="13" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3499,10 +3502,10 @@
       <c r="A82" t="s">
         <v>188</v>
       </c>
-      <c r="B82" s="27">
+      <c r="B82" s="16">
         <v>1</v>
       </c>
-      <c r="C82" s="24" t="s">
+      <c r="C82" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3510,10 +3513,10 @@
       <c r="A83" t="s">
         <v>189</v>
       </c>
-      <c r="B83" s="27">
+      <c r="B83" s="16">
         <v>0.2</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3521,10 +3524,10 @@
       <c r="A84" t="s">
         <v>190</v>
       </c>
-      <c r="B84" s="27">
+      <c r="B84" s="16">
         <v>0</v>
       </c>
-      <c r="C84" s="24" t="s">
+      <c r="C84" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3532,10 +3535,10 @@
       <c r="A85" t="s">
         <v>191</v>
       </c>
-      <c r="B85" s="27">
+      <c r="B85" s="16">
         <v>0.16</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3543,10 +3546,10 @@
       <c r="A86" t="s">
         <v>192</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B86" s="16">
         <v>0</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3554,10 +3557,10 @@
       <c r="A87" t="s">
         <v>193</v>
       </c>
-      <c r="B87" s="27">
+      <c r="B87" s="16">
         <v>0</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3565,10 +3568,10 @@
       <c r="A88" t="s">
         <v>194</v>
       </c>
-      <c r="B88" s="27">
+      <c r="B88" s="16">
         <v>0</v>
       </c>
-      <c r="C88" s="24" t="s">
+      <c r="C88" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3576,10 +3579,10 @@
       <c r="A89" t="s">
         <v>195</v>
       </c>
-      <c r="B89" s="27">
+      <c r="B89" s="16">
         <v>0.5</v>
       </c>
-      <c r="C89" s="24" t="s">
+      <c r="C89" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3587,10 +3590,10 @@
       <c r="A90" t="s">
         <v>196</v>
       </c>
-      <c r="B90" s="27">
+      <c r="B90" s="16">
         <v>1100</v>
       </c>
-      <c r="C90" s="24" t="s">
+      <c r="C90" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3598,10 +3601,10 @@
       <c r="A91" t="s">
         <v>197</v>
       </c>
-      <c r="B91" s="27">
+      <c r="B91" s="16">
         <v>0</v>
       </c>
-      <c r="C91" s="24" t="s">
+      <c r="C91" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3609,10 +3612,10 @@
       <c r="A92" t="s">
         <v>198</v>
       </c>
-      <c r="B92" s="27">
+      <c r="B92" s="16">
         <v>0</v>
       </c>
-      <c r="C92" s="24" t="s">
+      <c r="C92" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3620,10 +3623,10 @@
       <c r="A93" t="s">
         <v>199</v>
       </c>
-      <c r="B93" s="27">
+      <c r="B93" s="16">
         <v>20</v>
       </c>
-      <c r="C93" s="24" t="s">
+      <c r="C93" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3651,133 +3654,133 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="29" customWidth="1"/>
-    <col min="3" max="4" width="6.90625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="18" customWidth="1"/>
+    <col min="3" max="4" width="6.90625" style="18" customWidth="1"/>
     <col min="5" max="6" width="8.54296875" customWidth="1"/>
     <col min="7" max="7" width="8.36328125" customWidth="1"/>
     <col min="8" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
     </row>
     <row r="5" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
     </row>
     <row r="8" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="18" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="18">
         <v>1000</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="18">
         <v>1100</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="18">
         <v>100</v>
       </c>
     </row>
@@ -3809,237 +3812,237 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="29" customWidth="1"/>
-    <col min="4" max="5" width="15" style="29" customWidth="1"/>
-    <col min="6" max="7" width="9.36328125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" style="29" customWidth="1"/>
-    <col min="10" max="18" width="6.90625" style="29" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" style="29" customWidth="1"/>
-    <col min="20" max="20" width="11.08984375" style="29" customWidth="1"/>
-    <col min="21" max="1023" width="6.90625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="18" customWidth="1"/>
+    <col min="4" max="5" width="15" style="18" customWidth="1"/>
+    <col min="6" max="7" width="9.36328125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" style="18" customWidth="1"/>
+    <col min="10" max="18" width="6.90625" style="18" customWidth="1"/>
+    <col min="19" max="19" width="12.453125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="11.08984375" style="18" customWidth="1"/>
+    <col min="21" max="1023" width="6.90625" style="18" customWidth="1"/>
     <col min="1024" max="1025" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I2" s="20"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="24"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="24"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="24"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="24"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="24"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="24"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="24"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="24"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="24"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="24"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I13" s="20"/>
-      <c r="J13" s="24"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="L14" s="25"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="18" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4067,531 +4070,548 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMD38"/>
+  <dimension ref="A1:AMD39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6328125" customWidth="1"/>
-    <col min="2" max="4" width="13.08984375" style="29" customWidth="1"/>
-    <col min="5" max="1018" width="6.90625" style="29" customWidth="1"/>
+    <col min="2" max="4" width="13.08984375" style="18" customWidth="1"/>
+    <col min="5" max="1018" width="6.90625" style="18" customWidth="1"/>
     <col min="1019" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="41"/>
+      <c r="A2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="42"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
-        <v>250</v>
-      </c>
-      <c r="B9" s="43" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="123" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="35" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="34" t="s">
         <v>265</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C19" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="E19" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="47" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B19" s="47" t="s">
+      <c r="C34" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C37" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="B20" s="47" t="s">
+      <c r="D37" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="B38" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>268</v>
-      </c>
-      <c r="B21" s="47" t="s">
+      <c r="C38" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="D38" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="E38" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
-        <v>269</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
-        <v>270</v>
-      </c>
-      <c r="B23" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
-        <v>271</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
-        <v>272</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
-        <v>273</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
-        <v>274</v>
-      </c>
-      <c r="B27" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D28" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
-        <v>276</v>
-      </c>
-      <c r="B29" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
-        <v>277</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="E30" s="47" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>279</v>
-      </c>
-      <c r="B31" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="E31" s="47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
-        <v>280</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="B34" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
-        <v>255</v>
-      </c>
-      <c r="B35" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D35" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
-        <v>257</v>
-      </c>
-      <c r="B36" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
-        <v>259</v>
-      </c>
-      <c r="B37" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="E37" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="47"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="F38" s="36"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B39" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C39" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D39" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E39" s="38" t="s">
         <v>284</v>
       </c>
     </row>
@@ -4630,499 +4650,499 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="50"/>
+      <c r="A2" s="39"/>
     </row>
     <row r="3" spans="1:8" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="67" t="s">
         <v>289</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="67" t="s">
         <v>291</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="40" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="65" t="s">
         <v>293</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="40" t="s">
         <v>294</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="65" t="s">
         <v>295</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="65" t="s">
         <v>297</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="41" t="s">
         <v>298</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="42" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="43">
         <v>0.28622953868737899</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="43">
         <v>0.25807310904584102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="43" t="s">
         <v>302</v>
       </c>
-      <c r="B13" s="54">
+      <c r="B13" s="43">
         <v>0.23396226376115001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="43" t="s">
         <v>303</v>
       </c>
-      <c r="B14" s="54">
+      <c r="B14" s="43">
         <v>0.22173508850563001</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="70" t="s">
         <v>304</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="45" t="s">
         <v>305</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="47" t="s">
         <v>299</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="44" t="s">
         <v>307</v>
       </c>
-      <c r="G17" s="55" t="s">
+      <c r="G17" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="44" t="s">
         <v>309</v>
       </c>
-      <c r="I17" s="55" t="s">
+      <c r="I17" s="44" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="71" t="s">
         <v>311</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="49" t="s">
         <v>313</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="50">
         <v>0.51388888888888895</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="63" t="s">
+      <c r="E18" s="51"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="64" t="s">
+      <c r="A19" s="71"/>
+      <c r="B19" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="54" t="s">
         <v>316</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="55">
         <v>0.48611111111111099</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="63" t="s">
+      <c r="E19" s="51"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="48" t="s">
         <v>318</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="49" t="s">
         <v>319</v>
       </c>
-      <c r="D20" s="61">
+      <c r="D20" s="50">
         <v>0.25987103174603199</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="63" t="s">
+      <c r="E20" s="51"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="67" t="s">
+      <c r="A21" s="71"/>
+      <c r="B21" s="56" t="s">
         <v>320</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="43" t="s">
         <v>321</v>
       </c>
-      <c r="D21" s="68">
+      <c r="D21" s="57">
         <v>0.23849206349206301</v>
       </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="63" t="s">
+      <c r="E21" s="51"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="67" t="s">
+      <c r="A22" s="71"/>
+      <c r="B22" s="56" t="s">
         <v>322</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="43" t="s">
         <v>323</v>
       </c>
-      <c r="D22" s="68">
+      <c r="D22" s="57">
         <v>0.246825396825397</v>
       </c>
-      <c r="E22" s="69">
+      <c r="E22" s="58">
         <v>2.75</v>
       </c>
-      <c r="F22" s="63" t="s">
+      <c r="F22" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G22" s="63">
+      <c r="G22" s="52">
         <v>1.88</v>
       </c>
-      <c r="H22" s="63">
+      <c r="H22" s="52">
         <v>3</v>
       </c>
-      <c r="I22" s="63" t="s">
+      <c r="I22" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="64" t="s">
+      <c r="A23" s="71"/>
+      <c r="B23" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="54" t="s">
         <v>325</v>
       </c>
-      <c r="D23" s="66">
+      <c r="D23" s="55">
         <v>0.25481150793650797</v>
       </c>
-      <c r="E23" s="69">
+      <c r="E23" s="58">
         <v>2.25</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="F23" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G23" s="63">
+      <c r="G23" s="52">
         <v>1.5</v>
       </c>
-      <c r="H23" s="63">
+      <c r="H23" s="52">
         <v>3</v>
       </c>
-      <c r="I23" s="63" t="s">
+      <c r="I23" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="72" t="s">
         <v>326</v>
       </c>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="59" t="s">
         <v>327</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="43" t="s">
         <v>328</v>
       </c>
-      <c r="D24" s="68">
+      <c r="D24" s="57">
         <v>0.26535443722943702</v>
       </c>
-      <c r="E24" s="69">
+      <c r="E24" s="58">
         <v>2</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G24" s="63">
+      <c r="G24" s="52">
         <v>2.6</v>
       </c>
-      <c r="H24" s="63">
+      <c r="H24" s="52">
         <v>2.17</v>
       </c>
-      <c r="I24" s="63" t="s">
+      <c r="I24" s="52" t="s">
         <v>329</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="N24" s="68"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="70" t="s">
+      <c r="A25" s="72"/>
+      <c r="B25" s="59" t="s">
         <v>330</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="43" t="s">
         <v>331</v>
       </c>
-      <c r="D25" s="68">
+      <c r="D25" s="57">
         <v>0.39644209956710003</v>
       </c>
-      <c r="E25" s="62"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="63" t="s">
+      <c r="E25" s="51"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="52" t="s">
         <v>314</v>
       </c>
-      <c r="N25" s="2"/>
+      <c r="N25" s="68"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="71" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="60" t="s">
         <v>332</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="54" t="s">
         <v>333</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="55">
         <v>0.33820346320346301</v>
       </c>
-      <c r="E26" s="69">
+      <c r="E26" s="58">
         <v>2.57</v>
       </c>
-      <c r="F26" s="63" t="s">
+      <c r="F26" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="63">
+      <c r="G26" s="52">
         <v>1.71</v>
       </c>
-      <c r="H26" s="63">
+      <c r="H26" s="52">
         <v>2.14</v>
       </c>
-      <c r="I26" s="63" t="s">
+      <c r="I26" s="52" t="s">
         <v>329</v>
       </c>
-      <c r="N26" s="2"/>
+      <c r="N26" s="68"/>
     </row>
     <row r="27" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="69" t="s">
         <v>334</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="61" t="s">
         <v>335</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="49" t="s">
         <v>336</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="50">
         <v>0.25580808080808098</v>
       </c>
-      <c r="E27" s="69">
+      <c r="E27" s="58">
         <v>0</v>
       </c>
-      <c r="F27" s="63" t="s">
+      <c r="F27" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G27" s="63">
+      <c r="G27" s="52">
         <v>0.77</v>
       </c>
-      <c r="H27" s="63">
+      <c r="H27" s="52">
         <v>0.44</v>
       </c>
-      <c r="I27" s="63" t="s">
+      <c r="I27" s="52" t="s">
         <v>314</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="J27" s="14" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="70" t="s">
+      <c r="A28" s="69"/>
+      <c r="B28" s="59" t="s">
         <v>338</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="43" t="s">
         <v>339</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="57">
         <v>0.38377525252525302</v>
       </c>
-      <c r="E28" s="69">
+      <c r="E28" s="58">
         <v>2.63</v>
       </c>
-      <c r="F28" s="63" t="s">
+      <c r="F28" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="63">
+      <c r="G28" s="52">
         <v>1</v>
       </c>
-      <c r="H28" s="63">
+      <c r="H28" s="52">
         <v>1.88</v>
       </c>
-      <c r="I28" s="63" t="s">
+      <c r="I28" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="71" t="s">
+      <c r="A29" s="69"/>
+      <c r="B29" s="60" t="s">
         <v>340</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="54" t="s">
         <v>341</v>
       </c>
-      <c r="D29" s="66">
+      <c r="D29" s="55">
         <v>0.360416666666667</v>
       </c>
-      <c r="E29" s="69">
+      <c r="E29" s="58">
         <v>1.63</v>
       </c>
-      <c r="F29" s="63" t="s">
+      <c r="F29" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G29" s="63">
+      <c r="G29" s="52">
         <v>1.5</v>
       </c>
-      <c r="H29" s="63">
+      <c r="H29" s="52">
         <v>2.63</v>
       </c>
-      <c r="I29" s="63" t="s">
+      <c r="I29" s="52" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="70" t="s">
         <v>296</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="70"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="44" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="44" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="str">
+      <c r="A34" s="43" t="str">
         <f>IF(input_sensitivity!A11 = "","",input_sensitivity!A11)</f>
         <v>pv_cost_investment</v>
       </c>
-      <c r="B34" s="54" t="b">
+      <c r="B34" s="43" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>